<commit_message>
Modification du journa de travail
</commit_message>
<xml_diff>
--- a/doc/Journal de Travail.xlsx
+++ b/doc/Journal de Travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TPI\TPI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68B39EA-3AAD-402C-8132-18ACC42C7CD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88754323-C099-4797-A026-31FA35DA9F51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30705" yWindow="255" windowWidth="26850" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Feature Team</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>Création des Readme pour le github</t>
+  </si>
+  <si>
+    <t>Remise en forme du journal de travail ainsi que les taches effectuer durant la journée</t>
+  </si>
+  <si>
+    <t>Travail effectuer durant la journée</t>
   </si>
 </sst>
 </file>
@@ -131,7 +143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\.mm\.yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -268,18 +280,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -288,16 +296,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -592,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,45 +614,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -714,7 +718,7 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
@@ -735,7 +739,7 @@
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
         <v>27</v>
       </c>
@@ -756,126 +760,163 @@
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>44257</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>44257</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>44257</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>44257</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>44257</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="A14" s="5">
+        <v>44257</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>44257</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Documentation mise a jour
</commit_message>
<xml_diff>
--- a/doc/Journal de Travail.xlsx
+++ b/doc/Journal de Travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TPI\TPI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88754323-C099-4797-A026-31FA35DA9F51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB8B364-3B7A-4DAE-84C2-344B7FC36CC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30705" yWindow="255" windowWidth="26850" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Redaction du journal de travail</t>
   </si>
   <si>
-    <t>React native</t>
-  </si>
-  <si>
     <t>2h</t>
   </si>
   <si>
@@ -136,6 +133,30 @@
   </si>
   <si>
     <t>Travail effectuer durant la journée</t>
+  </si>
+  <si>
+    <t>React native (Frontend)</t>
+  </si>
+  <si>
+    <t>Référance (sur le git)</t>
+  </si>
+  <si>
+    <t>doc/Maquette app.pdf</t>
+  </si>
+  <si>
+    <t>front_mobile/chibre-manager/src/screen/Home</t>
+  </si>
+  <si>
+    <t>front_mobile/chibre-manager/src/screen/Game</t>
+  </si>
+  <si>
+    <t>front_mobile/chibre-manager/src/screen/CreateGame</t>
+  </si>
+  <si>
+    <t>doc/schéma ERD.svg</t>
+  </si>
+  <si>
+    <t>backend_api/chibre-manager/db/migrate/</t>
   </si>
 </sst>
 </file>
@@ -596,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,12 +629,13 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="62.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="78.5703125" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -623,8 +645,9 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -632,8 +655,9 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -653,10 +677,13 @@
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44256</v>
       </c>
@@ -676,10 +703,11 @@
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44256</v>
       </c>
@@ -699,10 +727,13 @@
         <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44256</v>
       </c>
@@ -720,10 +751,13 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44256</v>
       </c>
@@ -741,10 +775,13 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44256</v>
       </c>
@@ -761,124 +798,140 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>44257</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>44257</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>44257</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>44257</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>44257</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>44257</v>
       </c>
@@ -886,18 +939,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>44257</v>
       </c>
@@ -905,22 +959,23 @@
         <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
document mis a jour
</commit_message>
<xml_diff>
--- a/doc/Journal de Travail.xlsx
+++ b/doc/Journal de Travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TPI\TPI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6AA2ED-06CF-4221-88C4-BC6A3F59A907}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5FABDA-B25F-4AA0-B246-F10C23EFE6DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31170" yWindow="30" windowWidth="29940" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="103">
   <si>
     <t>Date</t>
   </si>
@@ -310,6 +310,30 @@
   </si>
   <si>
     <t>Mise a jour des models pour les relation annonces player et player_annonces</t>
+  </si>
+  <si>
+    <t>Feature - Calcule des points</t>
+  </si>
+  <si>
+    <t>Feature - Qui commence ?</t>
+  </si>
+  <si>
+    <t>Feature - Atout de la partie ?</t>
+  </si>
+  <si>
+    <t>Mise a jour controller Game</t>
+  </si>
+  <si>
+    <t>Permet de calculer les points de chaque equipe et de renvoyer les points sur le serveur web</t>
+  </si>
+  <si>
+    <t>Permet de savoir qui doit commencer et choisir l'atout</t>
+  </si>
+  <si>
+    <t>Permet de savoir quel atout est présent pour la manche</t>
+  </si>
+  <si>
+    <t>Mise  a jour du controller pour les manche et l'atout d'une partie</t>
   </si>
 </sst>
 </file>
@@ -491,15 +515,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -788,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,26 +831,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1560,7 +1584,7 @@
       <c r="G31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="8" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1586,7 +1610,7 @@
       <c r="G32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="8" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1612,7 +1636,7 @@
       <c r="G33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="8" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1636,9 +1660,105 @@
       <c r="G34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H34" s="8" t="s">
         <v>91</v>
       </c>
+    </row>
+    <row r="35" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>44263</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>44263</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>44263</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>44263</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Mise a jours des documents
</commit_message>
<xml_diff>
--- a/doc/Journal de Travail.xlsx
+++ b/doc/Journal de Travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TPI\TPI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FC654B-E742-4359-BFA4-0CA77E6F10D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBED54E3-D28B-4D61-A9B7-D968EC602E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="2025" windowWidth="21225" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="130">
   <si>
     <t>Date</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Permet d'avoir accès a l'API n'importe ou</t>
+  </si>
+  <si>
+    <t>Mise a jour du rapport de travail</t>
+  </si>
+  <si>
+    <t>Test de l'application</t>
   </si>
 </sst>
 </file>
@@ -887,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,6 +2074,50 @@
         <v>24</v>
       </c>
       <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>44267</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>44267</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>